<commit_message>
changes in summary and Transcriptanalysis
changed filtered seurat objects (human/mouse)
changed celltypeidentification after cellfiltering for human (script/summary)
added celltypeidentification after cellfiltering for mouse in summary
added comments to summary
chnaged control to untreaded in plot titles
</commit_message>
<xml_diff>
--- a/ProjectTransferSCRnaSeq.xlsx
+++ b/ProjectTransferSCRnaSeq.xlsx
@@ -1,14 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PI3K\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF1D9E1-6F8B-4B36-BF17-78340BAB0C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Positive" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Negative" sheetId="2" r:id="rId5"/>
+    <sheet name="Positive" sheetId="1" r:id="rId1"/>
+    <sheet name="Negative" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjBgCmCTwcmKtMuE3YhoPil5c/7sw=="/>
     </ext>
@@ -17,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="138">
   <si>
     <t>Part</t>
   </si>
@@ -159,17 +179,18 @@
   <si>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
-        <color theme="1"/>
       </rPr>
       <t>S</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
       </rPr>
       <t>ample Tag Demultiplexing</t>
     </r>
@@ -422,60 +443,115 @@
   </si>
   <si>
     <t>/PI3K/CelltypeIdentification/otherMethods/Clusterannotation_mouse_otherMethods.Rmd</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>BIH-Cluster</t>
+  </si>
+  <si>
+    <t>SODAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIH-Cluster/SODAR/github </t>
+  </si>
+  <si>
+    <t>BIH-Cluster/SODAR/github</t>
+  </si>
+  <si>
+    <t>BIH-Cluster/SODAR</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Alignment of the treated part from the HN11097 xenograft with BD sample tags to the human reference genome hg38 -&gt; Error in alignment step of the BD rhapsody pipeline ("Couldn´t read in the reference genome proberly due to missing information")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;docs-Calibri&quot;"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -483,66 +559,54 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -732,28 +796,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="49.57"/>
-    <col customWidth="1" min="2" max="3" width="41.0"/>
-    <col customWidth="1" min="4" max="4" width="125.71"/>
-    <col customWidth="1" min="5" max="5" width="167.71"/>
-    <col customWidth="1" min="6" max="6" width="78.86"/>
-    <col customWidth="1" min="7" max="27" width="8.71"/>
+    <col min="1" max="1" width="49.54296875" customWidth="1"/>
+    <col min="2" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="125.7265625" customWidth="1"/>
+    <col min="5" max="5" width="167.7265625" customWidth="1"/>
+    <col min="6" max="6" width="78.81640625" customWidth="1"/>
+    <col min="7" max="7" width="35.08984375" customWidth="1"/>
+    <col min="8" max="27" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:7" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,417 +839,486 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="C3" s="3" t="s">
+      <c r="G2" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.25" customHeight="1">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+      <c r="G3" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5" t="s">
+      <c r="G4" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5" t="s">
+      <c r="G5" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="G6" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="B8" s="5" t="s">
+      <c r="G7" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.25" customHeight="1">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="B9" s="5" t="s">
+      <c r="G8" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.25" customHeight="1">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+      <c r="G9" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="2" t="s">
+      <c r="G10" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="3" t="s">
+      <c r="G11" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+      <c r="G12" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.25" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="G13" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="2" t="s">
+      <c r="G14" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
+      <c r="G15" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="2" t="s">
+      <c r="G16" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="B18" s="5"/>
-      <c r="D18" s="5" t="s">
+      <c r="G17" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.25" customHeight="1">
+      <c r="B18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="B19" s="5" t="s">
+      <c r="G18" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.25" customHeight="1">
+      <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="8" t="s">
+      <c r="G19" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A20" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="8" t="s">
+      <c r="G20" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="B22" s="5" t="s">
+      <c r="G21" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.25" customHeight="1">
+      <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="8" t="s">
+      <c r="G22" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+      <c r="G23" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2157,395 +2293,450 @@
     <row r="1004" ht="14.25" customHeight="1"/>
     <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="52.57"/>
-    <col customWidth="1" min="2" max="3" width="46.43"/>
-    <col customWidth="1" min="4" max="4" width="456.0"/>
-    <col customWidth="1" min="5" max="5" width="170.14"/>
-    <col customWidth="1" min="6" max="6" width="78.86"/>
-    <col customWidth="1" min="7" max="27" width="8.71"/>
+    <col min="1" max="1" width="52.54296875" customWidth="1"/>
+    <col min="2" max="3" width="46.453125" customWidth="1"/>
+    <col min="4" max="4" width="456" customWidth="1"/>
+    <col min="5" max="5" width="170.08984375" customWidth="1"/>
+    <col min="6" max="6" width="81.54296875" customWidth="1"/>
+    <col min="7" max="7" width="35.08984375" customWidth="1"/>
+    <col min="8" max="8" width="26.26953125" customWidth="1"/>
+    <col min="9" max="27" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.25" customHeight="1">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="B3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5" t="s">
+      <c r="G4" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5" t="s">
+      <c r="G5" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="G6" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="B8" s="5" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A8" s="1"/>
+      <c r="B8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.25" customHeight="1">
+      <c r="B9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="B9" s="5" t="s">
+      <c r="G9" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14.25" customHeight="1">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="B10" s="5" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" ht="14.25" customHeight="1">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F12" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5" t="s">
+      <c r="G12" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F13" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="G13" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E14" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F14" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="2"/>
-      <c r="B14" s="5" t="s">
+      <c r="G14" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D15" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E15" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F15" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="2" t="s">
+      <c r="G15" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E16" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F16" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5" t="s">
+      <c r="G16" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E17" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F17" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="2" t="s">
+      <c r="G17" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D18" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E18" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F18" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="B18" s="5" t="s">
+      <c r="G18" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.25" customHeight="1">
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E19" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F19" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="B19" s="5" t="s">
+      <c r="G19" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.25" customHeight="1">
+      <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E20" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F20" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="B20" s="5" t="s">
+      <c r="G20" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.25" customHeight="1">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D21" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E21" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F21" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+      <c r="G21" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -3519,9 +3710,7 @@
     <row r="1003" ht="14.25" customHeight="1"/>
     <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>